<commit_message>
Tabulky a grafy done
</commit_message>
<xml_diff>
--- a/Uloha5/charakteristika.xlsx
+++ b/Uloha5/charakteristika.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vutbr-my.sharepoint.com/personal/247759_vutbr_cz/Documents/Bc. 5. Semestr/BPC-MVAA/BPC-MVAA-Protokoly-2024/Uloha5/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="8_{8EEF8497-A05D-4273-AE3E-00BA78E0CE53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F492016F-2ECE-4123-BCD8-251B3B97B558}"/>
+  <xr:revisionPtr revIDLastSave="13" documentId="8_{8EEF8497-A05D-4273-AE3E-00BA78E0CE53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1247AD75-A4ED-4B0E-B538-495CA4E69E5C}"/>
   <bookViews>
-    <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14169" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="1536" yWindow="384" windowWidth="30720" windowHeight="16272" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>Kmitočet</t>
   </si>
@@ -170,10 +170,6 @@
     </r>
   </si>
   <si>
-    <t>Napětí na výstupu zesilovače
-rezistoru</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <i/>
@@ -217,6 +213,13 @@
   <si>
     <t>Fáze
 přenosu</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Napětí na výstupu zesilovače
+</t>
   </si>
 </sst>
 </file>
@@ -2498,27 +2501,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.75" style="19" customWidth="1"/>
-    <col min="2" max="2" width="18.75" customWidth="1"/>
-    <col min="3" max="3" width="18.75" style="13" customWidth="1"/>
-    <col min="4" max="4" width="18.75" customWidth="1"/>
-    <col min="5" max="5" width="48.375" customWidth="1"/>
-    <col min="8" max="8" width="9.125" customWidth="1"/>
+    <col min="1" max="1" width="18.77734375" style="19" customWidth="1"/>
+    <col min="2" max="2" width="18.77734375" customWidth="1"/>
+    <col min="3" max="3" width="18.77734375" style="13" customWidth="1"/>
+    <col min="4" max="4" width="18.77734375" customWidth="1"/>
+    <col min="5" max="5" width="48.33203125" customWidth="1"/>
+    <col min="8" max="8" width="9.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="23.8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:8" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A1" s="18" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15.8" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:8" ht="42.8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="20" t="s">
         <v>0</v>
       </c>
@@ -2526,22 +2527,22 @@
         <v>3</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="H3" s="5"/>
     </row>
-    <row r="4" spans="1:8" ht="17" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A4" s="21" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C4" s="15" t="s">
         <v>6</v>
@@ -2554,7 +2555,7 @@
       </c>
       <c r="H4" s="6"/>
     </row>
-    <row r="5" spans="1:8" ht="14.95" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="22">
         <v>5</v>
       </c>
@@ -2571,7 +2572,7 @@
         <v>-84</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="14.95" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="22">
         <v>7</v>
       </c>
@@ -2588,7 +2589,7 @@
         <v>-60.4</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="14.95" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="22">
         <v>10</v>
       </c>
@@ -2606,7 +2607,7 @@
       </c>
       <c r="H7" s="7"/>
     </row>
-    <row r="8" spans="1:8" ht="14.95" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="22">
         <v>15</v>
       </c>
@@ -2624,7 +2625,7 @@
       </c>
       <c r="H8" s="7"/>
     </row>
-    <row r="9" spans="1:8" ht="14.95" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="23">
         <v>20</v>
       </c>
@@ -2641,7 +2642,7 @@
         <v>-22.4</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="14.95" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="23">
         <v>30</v>
       </c>
@@ -2658,7 +2659,7 @@
         <v>-14.6</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="14.95" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="23">
         <v>40</v>
       </c>
@@ -2675,7 +2676,7 @@
         <v>-12.7</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="14.95" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="23">
         <v>60</v>
       </c>
@@ -2692,7 +2693,7 @@
         <v>-6.5</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="14.95" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="23">
         <v>100</v>
       </c>
@@ -2709,7 +2710,7 @@
         <v>-3.9</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="14.95" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="23">
         <v>200</v>
       </c>
@@ -2726,7 +2727,7 @@
         <v>-2.8</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="14.95" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="23">
         <v>400</v>
       </c>
@@ -2743,7 +2744,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="14.95" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="23">
         <v>600</v>
       </c>
@@ -2760,7 +2761,7 @@
         <v>-1.8</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="14.95" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="23">
         <v>1000</v>
       </c>
@@ -2777,7 +2778,7 @@
         <v>-1.7</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="23">
         <v>2000</v>
       </c>
@@ -2794,7 +2795,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="23">
         <v>3000</v>
       </c>
@@ -2811,7 +2812,7 @@
         <v>-0.9</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="23">
         <v>4000</v>
       </c>
@@ -2828,7 +2829,7 @@
         <v>-1.2</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="23">
         <v>6000</v>
       </c>
@@ -2845,7 +2846,7 @@
         <v>-0.2</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="23">
         <v>10000</v>
       </c>
@@ -2862,7 +2863,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="23">
         <v>15000</v>
       </c>
@@ -2879,7 +2880,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="23">
         <v>20000</v>
       </c>
@@ -2896,7 +2897,7 @@
         <v>2.1</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="23">
         <v>30000</v>
       </c>
@@ -2913,7 +2914,7 @@
         <v>5.4</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="23">
         <v>40000</v>
       </c>
@@ -2930,7 +2931,7 @@
         <v>18.2</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="24">
         <v>60000</v>
       </c>
@@ -2947,7 +2948,7 @@
         <v>46.3</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="24">
         <v>100000</v>
       </c>
@@ -2964,7 +2965,7 @@
         <v>80.900000000000006</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="24">
         <v>150000</v>
       </c>
@@ -2981,7 +2982,7 @@
         <v>95.2</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="24">
         <v>200000</v>
       </c>
@@ -2998,7 +2999,7 @@
         <v>105.5</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="24">
         <v>300000</v>
       </c>
@@ -3015,7 +3016,7 @@
         <v>118.2</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="24">
         <v>400000</v>
       </c>
@@ -3032,7 +3033,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="24">
         <v>550000</v>
       </c>
@@ -3049,7 +3050,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="24">
         <v>600000</v>
       </c>
@@ -3066,7 +3067,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="24">
         <v>700000</v>
       </c>
@@ -3079,12 +3080,12 @@
       <c r="D35" s="8">
         <v>-10.8998611914182</v>
       </c>
-      <c r="E35" s="11">
-        <v>9.8999999999999899E+37</v>
+      <c r="E35" s="11" t="s">
+        <v>10</v>
       </c>
       <c r="F35" s="26"/>
     </row>
-    <row r="36" spans="1:6" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="25">
         <v>800000</v>
       </c>
@@ -3097,11 +3098,11 @@
       <c r="D36" s="9">
         <v>-11.397506159131201</v>
       </c>
-      <c r="E36" s="12">
-        <v>9.8999999999999899E+37</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E36" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D37" s="27">
         <f>MAX(D5:D36)</f>
         <v>8.7286833190089208</v>

</xml_diff>